<commit_message>
izgara firin ve mutfak sayfaları güncellendi bazı hatalar giderildi
</commit_message>
<xml_diff>
--- a/admin/gunluk_rapor.xlsx
+++ b/admin/gunluk_rapor.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Tarih</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>2024-07-20</t>
+  </si>
+  <si>
+    <t>2024-07-24</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +435,26 @@
         <v>1796</v>
       </c>
     </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
yeni bir lokanta sayfası eklendi , gerekli düznlemeler yapıldı
</commit_message>
<xml_diff>
--- a/admin/gunluk_rapor.xlsx
+++ b/admin/gunluk_rapor.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Tarih</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>2024-08-05</t>
+  </si>
+  <si>
+    <t>08/08/2024 15:23</t>
+  </si>
+  <si>
+    <t>08/08/2024 19:24</t>
   </si>
 </sst>
 </file>
@@ -393,7 +399,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +565,49 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3753</v>
+      </c>
+      <c r="D9">
+        <v>4170.0</v>
+      </c>
+      <c r="E9">
+        <v>417.0</v>
+      </c>
+      <c r="F9">
+        <v>3753</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>